<commit_message>
Processing on ARTY down from 7.74sec to 1.92s by optimizing mem access. Added statistics on memory access.
</commit_message>
<xml_diff>
--- a/src/fpgaPlayground/AFAMem/docs/SpeedTests-memcpy.xlsx
+++ b/src/fpgaPlayground/AFAMem/docs/SpeedTests-memcpy.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Size</t>
   </si>
@@ -126,23 +127,65 @@
     <t>Simple loop with two inner for-loops (array, read- and write-burst inferred)</t>
   </si>
   <si>
-    <t>AFAProcessing (Philipps data)</t>
-  </si>
-  <si>
     <t>0.2001</t>
   </si>
   <si>
-    <t>Dataset</t>
-  </si>
-  <si>
     <t>Unoptimized AFA; Iter#0</t>
+  </si>
+  <si>
+    <t>0.3000</t>
+  </si>
+  <si>
+    <t>0.3001</t>
+  </si>
+  <si>
+    <t>Optimized (adaptNetwork_HW: SRC and DST from Blockram, searchBestMatchComplete_HW: BlockRam)</t>
+  </si>
+  <si>
+    <t>Optimized (adaptNetwork_HW: SRC and DST from Blockram)</t>
+  </si>
+  <si>
+    <t>Optimized (adaptNetwork_HW: SRC from Blockram)</t>
+  </si>
+  <si>
+    <t>AFAProcessing (100 Spectra, Philipps data)</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>memAccess_AFAProcess_HW</t>
+  </si>
+  <si>
+    <t>memAccess_adaptNetwork_HW_read</t>
+  </si>
+  <si>
+    <t>memAccess_adaptNetwork_HW_write</t>
+  </si>
+  <si>
+    <t>memAccess_searchBestMatchComplete_HW</t>
+  </si>
+  <si>
+    <t>SW Version</t>
+  </si>
+  <si>
+    <t>0.3004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +195,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -176,10 +226,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,12 +244,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:L23"/>
+  <dimension ref="C2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -513,39 +574,39 @@
     <col min="4" max="4" width="7.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.1328125" customWidth="1"/>
-    <col min="7" max="7" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="54.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.45">
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="5" spans="3:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="6"/>
+      <c r="J5" s="10"/>
       <c r="K5" s="1"/>
       <c r="L5" s="2" t="s">
         <v>6</v>
@@ -760,17 +821,17 @@
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.45">
-      <c r="D17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="D17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C20" s="2"/>
@@ -779,42 +840,46 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="6" t="s">
+      <c r="G20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="10"/>
       <c r="K20" s="5"/>
       <c r="L20" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.45">
-      <c r="C21" s="2" t="s">
+    <row r="21" spans="3:12" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
+      <c r="G21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="H21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="I21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C22">
@@ -824,25 +889,29 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" t="s">
         <v>18</v>
       </c>
-      <c r="G22">
-        <v>100</v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3">
+      <c r="G22" s="3">
         <v>7736</v>
       </c>
-      <c r="J22" s="4">
-        <f>I22/1000</f>
+      <c r="H22" s="4">
+        <f>G22/1000</f>
         <v>7.7359999999999998</v>
+      </c>
+      <c r="I22" s="7">
+        <f>$H$22/H22</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="8">
+        <f>I22</f>
+        <v>1</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.45">
@@ -854,21 +923,103 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="G23" s="3">
+        <v>7160</v>
+      </c>
+      <c r="H23" s="4">
+        <f>G23/1000</f>
+        <v>7.16</v>
+      </c>
+      <c r="I23" s="7">
+        <f>$H$22/H23</f>
+        <v>1.0804469273743016</v>
+      </c>
+      <c r="J23" s="8">
+        <f>I23</f>
+        <v>1.0804469273743016</v>
+      </c>
+      <c r="L23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C24">
+        <f>C23+1</f>
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4041</v>
+      </c>
+      <c r="H24" s="4">
+        <f>G24/1000</f>
+        <v>4.0410000000000004</v>
+      </c>
+      <c r="I24" s="7">
+        <f>$H$22/H24</f>
+        <v>1.9143776292996781</v>
+      </c>
+      <c r="J24" s="8">
+        <f>I24</f>
+        <v>1.9143776292996781</v>
+      </c>
+      <c r="L24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C25">
+        <f>C24+1</f>
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1918</v>
+      </c>
+      <c r="H25" s="4">
+        <f>G25/1000</f>
+        <v>1.9179999999999999</v>
+      </c>
+      <c r="I25" s="7">
+        <f>$H$22/H25</f>
+        <v>4.0333680917622523</v>
+      </c>
+      <c r="J25" s="8">
+        <f>I25</f>
+        <v>4.0333680917622523</v>
+      </c>
+      <c r="L25" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="D17:L17"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -877,6 +1028,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B8:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="36.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2400</v>
+      </c>
+      <c r="D9" s="12">
+        <f>C9/1024^2</f>
+        <v>2.288818359375E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3">
+        <v>26564000</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" ref="D10:D12" si="0">C10/1024^2</f>
+        <v>25.333404541015625</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3">
+        <v>26380800</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>25.15869140625</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3">
+        <v>17495600</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>16.685104370117188</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Another factor 3.8 gained :-) Pipelining enabled: Now at 1529% @ ARTY
</commit_message>
<xml_diff>
--- a/src/fpgaPlayground/AFAMem/docs/SpeedTests-memcpy.xlsx
+++ b/src/fpgaPlayground/AFAMem/docs/SpeedTests-memcpy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Size</t>
   </si>
@@ -177,13 +177,31 @@
   <si>
     <t>0.3004</t>
   </si>
+  <si>
+    <t>#Samples</t>
+  </si>
+  <si>
+    <t>memAccess_adaptNetwork_HW_read (src1)</t>
+  </si>
+  <si>
+    <t>memAccess_adaptNetwork_HW_read (src2)</t>
+  </si>
+  <si>
+    <t>ExecutionTime</t>
+  </si>
+  <si>
+    <t>0.3005</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="171" formatCode="#,##0&quot;b&quot;"/>
+    <numFmt numFmtId="172" formatCode="0&quot;MB&quot;"/>
+    <numFmt numFmtId="173" formatCode="0.00&quot;s&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -230,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,6 +275,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -562,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:L25"/>
+  <dimension ref="C2:L26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -989,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
         <v>18</v>
@@ -1010,6 +1031,39 @@
         <v>4.0333680917622523</v>
       </c>
       <c r="L25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C26">
+        <f>C25+1</f>
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="3">
+        <v>506</v>
+      </c>
+      <c r="H26" s="4">
+        <f>G26/1000</f>
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I26" s="7">
+        <f>$H$22/H26</f>
+        <v>15.288537549407113</v>
+      </c>
+      <c r="J26" s="8">
+        <f>I26</f>
+        <v>15.288537549407113</v>
+      </c>
+      <c r="L26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1029,79 +1083,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:D13"/>
+  <dimension ref="B9:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="14">
         <v>2400</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="15">
         <f>C9/1024^2</f>
         <v>2.288818359375E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="14">
         <v>26564000</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="15">
         <f t="shared" ref="D10:D12" si="0">C10/1024^2</f>
         <v>25.333404541015625</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="14">
         <v>26380800</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="15">
         <f t="shared" si="0"/>
         <v>25.15869140625</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="14">
         <v>17495600</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="15">
         <f t="shared" si="0"/>
         <v>16.685104370117188</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E12">
+        <f>C12/$D$14</f>
+        <v>9550</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3">
+        <v>458</v>
+      </c>
+      <c r="D14" s="14">
+        <f>C14*4</f>
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="14">
+        <f>C10-C11</f>
+        <v>183200</v>
+      </c>
+      <c r="D15">
+        <f>C15/$D$14</f>
+        <v>100</v>
+      </c>
+      <c r="E15" s="12">
+        <f>SQRT(D15)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="14">
+        <f>C10-C15</f>
+        <v>26380800</v>
+      </c>
+      <c r="D16">
+        <f>C16/$D$14</f>
+        <v>14400</v>
+      </c>
+      <c r="E16" s="12">
+        <f>SQRT(D16)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1.9179999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>